<commit_message>
Adding new tables of analysis
</commit_message>
<xml_diff>
--- a/MinneSearch/results.xlsx
+++ b/MinneSearch/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muppy\Documents\GitHub\minneapolis-a-star\roadnetwork_search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muppy\Documents\GitHub\minneapolis-a-star\MinneSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B327E92A-90BE-43D8-A87F-9524A117C622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4276872C-08F7-450C-96CE-BB08A361ED9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{2614F997-B5EA-4407-9B12-AE49FF4CAC3A}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="27">
   <si>
     <t>Uniform Cost</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>AVG OpenSet Size</t>
+  </si>
+  <si>
+    <t>STDev f(goal)</t>
+  </si>
+  <si>
+    <t>STDev Path Size</t>
+  </si>
+  <si>
+    <t>STDev ClosedSet Size</t>
+  </si>
+  <si>
+    <t>STDev OpenSet Size</t>
+  </si>
+  <si>
+    <t>Euclidean Differences</t>
+  </si>
+  <si>
+    <t>Diagonal Differences</t>
+  </si>
+  <si>
+    <t>Manhattan Differences</t>
+  </si>
+  <si>
+    <t>(Uni. Cost. H) - Heuristic</t>
+  </si>
+  <si>
+    <t>(Norm h) - (2x Weighted h)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +576,7 @@
   <dimension ref="A1:M141"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,11 +585,11 @@
     <col min="2" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -971,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -993,8 +1020,13 @@
       <c r="G12">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,6 +1048,21 @@
       <c r="G13">
         <v>32</v>
       </c>
+      <c r="I13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1039,6 +1086,25 @@
       <c r="G14">
         <v>25</v>
       </c>
+      <c r="I14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <f>_xlfn.STDEV.P(D13:D32)</f>
+        <v>968.89437967818651</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" ref="K14:M14" si="0">_xlfn.STDEV.P(E13:E32)</f>
+        <v>8.6804377769787617</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="0"/>
+        <v>252.16867370869048</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>12.532358118087753</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1062,6 +1128,25 @@
       <c r="G15">
         <v>6</v>
       </c>
+      <c r="I15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <f>_xlfn.STDEV.P(D33:D52)</f>
+        <v>1015.7304949477884</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" ref="K15:M15" si="1">_xlfn.STDEV.P(E33:E52)</f>
+        <v>7.8056069591031809</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="1"/>
+        <v>137.55845121256635</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5992732251045503</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1085,8 +1170,27 @@
       <c r="G16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3">
+        <f>_xlfn.STDEV.P(D53:D72)</f>
+        <v>1014.417490800322</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" ref="K16:M16" si="2">_xlfn.STDEV.P(E53:E72)</f>
+        <v>8.1786306922369345</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="2"/>
+        <v>132.9200887751735</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="2"/>
+        <v>9.1020602063488898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,8 +1212,27 @@
       <c r="G17">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <f>_xlfn.STDEV.P(D73:D92)</f>
+        <v>1067.4392396585588</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" ref="K17:M17" si="3">_xlfn.STDEV.P(E73:E92)</f>
+        <v>7.7935871073594862</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="3"/>
+        <v>132.03010073464307</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="3"/>
+        <v>10.046890066085126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,8 +1254,27 @@
       <c r="G18">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <f>_xlfn.STDEV.P(D93:D112)</f>
+        <v>1022.8206933816857</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" ref="K18:M18" si="4">_xlfn.STDEV.P(E93:E112)</f>
+        <v>8.4573932154062703</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="4"/>
+        <v>290.50118760514562</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="4"/>
+        <v>11.267098117971637</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1154,8 +1296,27 @@
       <c r="G19">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="3">
+        <f>_xlfn.STDEV.P(D113:D132)</f>
+        <v>1021.4192020091566</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ref="K19:M19" si="5">_xlfn.STDEV.P(E113:E132)</f>
+        <v>9.5229984773704555</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="5"/>
+        <v>267.92939368423168</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="5"/>
+        <v>10.615554625171498</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1177,8 +1338,27 @@
       <c r="G20">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="3">
+        <f>_xlfn.STDEV.P(D133:D152)</f>
+        <v>1035.7450250544568</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" ref="K20:M20" si="6">_xlfn.STDEV.P(E133:E152)</f>
+        <v>9.3094933625126277</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="6"/>
+        <v>265.88259731610032</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="6"/>
+        <v>9.7979589711327115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1381,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1223,8 +1403,13 @@
       <c r="G22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1246,8 +1431,23 @@
       <c r="G23">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1269,8 +1469,27 @@
       <c r="G24">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="3">
+        <f>J4-J5</f>
+        <v>-126.19427500000029</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" ref="K24:M24" si="7">K4-K5</f>
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="7"/>
+        <v>77.199999999999989</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="7"/>
+        <v>5.0500000000000007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1292,8 +1511,27 @@
       <c r="G25">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="3">
+        <f>J6-J7</f>
+        <v>-109.86127600000009</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" ref="K25:M25" si="8">K6-K7</f>
+        <v>0.54999999999999716</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="8"/>
+        <v>21.5</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" si="8"/>
+        <v>2.9499999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1315,8 +1553,27 @@
       <c r="G26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="3">
+        <f>J8-J9</f>
+        <v>-145.29135000000042</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ref="K26:M26" si="9">K8-K9</f>
+        <v>-1.3000000000000007</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="9"/>
+        <v>41.75</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" si="9"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1339,7 +1596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -1361,8 +1618,13 @@
       <c r="G28">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1384,8 +1646,23 @@
       <c r="G29">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -1407,8 +1684,27 @@
       <c r="G30">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <f>J$3-J4</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" ref="K30:M30" si="10">K$3-K4</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="10"/>
+        <v>389.00000000000006</v>
+      </c>
+      <c r="M30" s="3">
+        <f t="shared" si="10"/>
+        <v>-3.1500000000000021</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1430,8 +1726,27 @@
       <c r="G31">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" ref="J31:M31" si="11">J$3-J5</f>
+        <v>-126.19427500000029</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="shared" si="11"/>
+        <v>466.20000000000005</v>
+      </c>
+      <c r="M31" s="3">
+        <f t="shared" si="11"/>
+        <v>1.8999999999999986</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -1453,8 +1768,27 @@
       <c r="G32">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" ref="J32:M32" si="12">J$3-J6</f>
+        <v>-59.583239000000049</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="12"/>
+        <v>0.85000000000000142</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" si="12"/>
+        <v>446.95000000000005</v>
+      </c>
+      <c r="M32" s="3">
+        <f t="shared" si="12"/>
+        <v>0.14999999999999858</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -1476,8 +1810,27 @@
       <c r="G33">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" ref="J33:M33" si="13">J$3-J7</f>
+        <v>-169.44451500000014</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="13"/>
+        <v>1.3999999999999986</v>
+      </c>
+      <c r="L33" s="3">
+        <f t="shared" si="13"/>
+        <v>468.45000000000005</v>
+      </c>
+      <c r="M33" s="3">
+        <f t="shared" si="13"/>
+        <v>3.0999999999999979</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1499,8 +1852,27 @@
       <c r="G34">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" ref="J34:M34" si="14">J$3-J8</f>
+        <v>-6.8002749999996013</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="14"/>
+        <v>0.25</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="14"/>
+        <v>103.55000000000007</v>
+      </c>
+      <c r="M34" s="3">
+        <f t="shared" si="14"/>
+        <v>-5.7000000000000028</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1522,8 +1894,27 @@
       <c r="G35">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" ref="J35:M35" si="15">J$3-J9</f>
+        <v>-152.09162500000002</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="15"/>
+        <v>-1.0500000000000007</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="15"/>
+        <v>145.30000000000007</v>
+      </c>
+      <c r="M35" s="3">
+        <f t="shared" si="15"/>
+        <v>-4.9500000000000028</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -1546,7 +1937,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +1960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -1592,7 +1983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -1615,7 +2006,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +2029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
@@ -1661,7 +2052,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
@@ -1684,7 +2075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>2</v>
       </c>
@@ -1707,7 +2098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
@@ -1730,7 +2121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
@@ -1753,7 +2144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
@@ -1776,7 +2167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
@@ -1799,7 +2190,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>